<commit_message>
Added some more results and began discussion of fast and hot
</commit_message>
<xml_diff>
--- a/paper/scaling_results.xlsx
+++ b/paper/scaling_results.xlsx
@@ -79,10 +79,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,13 +121,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -444,7 +464,7 @@
   <dimension ref="A2:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -671,6 +691,9 @@
       <c r="C21">
         <v>31.3</v>
       </c>
+      <c r="D21">
+        <v>9.91</v>
+      </c>
       <c r="E21">
         <v>5.15</v>
       </c>
@@ -722,8 +745,20 @@
       <c r="A24" t="s">
         <v>12</v>
       </c>
+      <c r="B24">
+        <v>6.48</v>
+      </c>
       <c r="C24">
         <v>3.19</v>
+      </c>
+      <c r="D24">
+        <v>1.49</v>
+      </c>
+      <c r="E24">
+        <v>0.84</v>
+      </c>
+      <c r="F24">
+        <v>0.85</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -739,6 +774,12 @@
       <c r="D25">
         <v>1.54</v>
       </c>
+      <c r="E25">
+        <v>0.85</v>
+      </c>
+      <c r="F25">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
@@ -753,57 +794,61 @@
       <c r="D26">
         <v>1.6</v>
       </c>
+      <c r="E26">
+        <v>0.89</v>
+      </c>
+      <c r="F26">
+        <v>0.82</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>17</v>
       </c>
       <c r="B27">
-        <v>53.25</v>
+        <v>6.29</v>
       </c>
       <c r="C27">
-        <v>48.35</v>
+        <v>6.36</v>
       </c>
       <c r="D27">
-        <v>16.100000000000001</v>
+        <v>4.95</v>
+      </c>
+      <c r="E27">
+        <v>2.4300000000000002</v>
       </c>
       <c r="F27">
-        <v>2.86</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>15</v>
       </c>
-      <c r="C28">
-        <v>36.840000000000003</v>
-      </c>
-      <c r="D28">
-        <v>10.93</v>
-      </c>
-      <c r="E28">
-        <v>8.77</v>
-      </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>16</v>
       </c>
       <c r="B29">
-        <v>199.29</v>
+        <v>76.88</v>
+      </c>
+      <c r="C29">
+        <v>58.27</v>
       </c>
       <c r="D29">
-        <v>42.68</v>
+        <v>14.022</v>
       </c>
       <c r="E29">
-        <v>23.05</v>
+        <v>13.08</v>
       </c>
       <c r="F29">
-        <v>10.46</v>
+        <v>7.76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Some changes before resubmission
</commit_message>
<xml_diff>
--- a/paper/scaling_results.xlsx
+++ b/paper/scaling_results.xlsx
@@ -121,8 +121,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -141,7 +147,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -149,6 +155,9 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -156,6 +165,9 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,7 +500,7 @@
   <dimension ref="A2:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1014,19 +1026,19 @@
         <v>17</v>
       </c>
       <c r="B43">
-        <v>2.97</v>
+        <v>3.27</v>
       </c>
       <c r="C43">
-        <v>2.34</v>
+        <v>2.36</v>
       </c>
       <c r="D43">
-        <v>1.91</v>
+        <v>1.74</v>
       </c>
       <c r="E43">
-        <v>1.66</v>
+        <v>1.24</v>
       </c>
       <c r="F43">
-        <v>1.53</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1118,19 +1130,19 @@
       </c>
       <c r="C50">
         <f>$B43/C43</f>
-        <v>1.2692307692307694</v>
+        <v>1.3855932203389831</v>
       </c>
       <c r="D50">
         <f t="shared" si="0"/>
-        <v>1.554973821989529</v>
+        <v>1.8793103448275863</v>
       </c>
       <c r="E50">
         <f t="shared" si="0"/>
-        <v>1.7891566265060244</v>
+        <v>2.6370967741935485</v>
       </c>
       <c r="F50">
         <f t="shared" si="0"/>
-        <v>1.9411764705882353</v>
+        <v>4.2467532467532463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>